<commit_message>
Corrected scores to total 25 pts.
</commit_message>
<xml_diff>
--- a/proiect/tema_ISM_2023_2024.xlsx
+++ b/proiect/tema_ISM_2023_2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ISM\proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10DDA7A-C00F-4763-AF75-8EA61507BF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3E49FB-DEF0-4BE3-B735-5B15D8B56977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Tema</t>
   </si>
@@ -684,6 +673,9 @@
       </rPr>
       <t xml:space="preserve"> Saptamana 8, Duminica, ora 23:59</t>
     </r>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -825,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -855,6 +847,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,9 +867,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -913,7 +907,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1019,7 +1013,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1161,7 +1155,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,38 +1169,38 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1214,7 +1208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -1222,7 +1216,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
@@ -1230,7 +1224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
@@ -1239,77 +1233,77 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
@@ -1322,20 +1316,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3A509B-A0E3-4ECA-B1C9-A35229B531C9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" activeCellId="1" sqref="A14:XFD14 A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="132.88671875" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="132.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
@@ -1357,7 +1351,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -1368,7 +1362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -1379,18 +1373,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="11">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -1401,7 +1395,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1412,18 +1406,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="11">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>27</v>
       </c>
@@ -1434,18 +1428,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="13">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>29</v>
       </c>
@@ -1456,7 +1450,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>30</v>
       </c>
@@ -1467,16 +1461,26 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="13">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="15">
+        <f>SUM(B2:B13)</f>
+        <v>25</v>
+      </c>
+      <c r="C14" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Specificat nr de membri per echipa.
</commit_message>
<xml_diff>
--- a/proiect/tema_ISM_2023_2024.xlsx
+++ b/proiect/tema_ISM_2023_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ISM\proiect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ISM\proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3E49FB-DEF0-4BE3-B735-5B15D8B56977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0034E655-CCD8-49DD-918B-BDBCAEB6F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" activeTab="1" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Tema</t>
   </si>
@@ -676,6 +687,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Se vor constitui echipe de cate 2 studenti.</t>
   </si>
 </sst>
 </file>
@@ -727,7 +741,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -749,6 +763,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -847,8 +867,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,9 +888,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -907,7 +928,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1013,7 +1034,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1155,7 +1176,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1163,148 +1184,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB50FB3-F61C-47DF-9F9D-09B36B0EB91E}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A2:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="106.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B9" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B11" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="5">
-        <f t="shared" ref="B9" si="0">SUM(B6:B8)</f>
+      <c r="B12" s="5">
+        <f t="shared" ref="B12" si="0">SUM(B9:B11)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1318,18 +1344,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3A509B-A0E3-4ECA-B1C9-A35229B531C9}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="132.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="132.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>20</v>
       </c>
@@ -1351,7 +1377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -1362,7 +1388,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -1373,7 +1399,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -1384,7 +1410,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -1395,7 +1421,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1406,7 +1432,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>26</v>
       </c>
@@ -1417,7 +1443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
@@ -1439,7 +1465,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="13" t="s">
         <v>29</v>
       </c>
@@ -1450,7 +1476,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A12" s="13" t="s">
         <v>30</v>
       </c>
@@ -1461,7 +1487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
@@ -1472,7 +1498,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>50</v>
       </c>
@@ -1480,7 +1506,7 @@
         <f>SUM(B2:B13)</f>
         <v>25</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mentionat explicit ca PM si GM cerute sunt valorile minime.
</commit_message>
<xml_diff>
--- a/proiect/tema_ISM_2023_2024.xlsx
+++ b/proiect/tema_ISM_2023_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ISM\proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0034E655-CCD8-49DD-918B-BDBCAEB6F284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981EB71F-4DC9-4E02-AB65-E0BF64FBBFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="15196" activeTab="1" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4BB2D8F-7608-4556-B435-FC8A6F3F02EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -224,51 +213,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Margine de faza: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>60 deg (caz nominal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Margine de castig: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10 dB (caz nominal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tensiune de offset: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>+/- 20 mV (analiza Monte Carlo)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Temperatura: </t>
     </r>
     <r>
@@ -345,21 +289,6 @@
   </si>
   <si>
     <t>#3.5</t>
-  </si>
-  <si>
-    <r>
-      <t>Amplificare: 4</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0 dB (minim)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -690,6 +619,66 @@
   </si>
   <si>
     <t>Se vor constitui echipe de cate 2 studenti.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Margine de faza: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>60 deg (minim, in cazul nominal)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Margine de castig: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10 dB (minim, in cazul nominal)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tensiune de offset: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+/- 20 mV (maxim, in analiza Monte Carlo)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Amplificare: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>40 dB (minim)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -888,9 +877,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -928,7 +917,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1034,7 +1023,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1176,7 +1165,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1186,71 +1175,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB50FB3-F61C-47DF-9F9D-09B36B0EB91E}">
   <dimension ref="A2:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
@@ -1259,79 +1248,79 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1344,18 +1333,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3A509B-A0E3-4ECA-B1C9-A35229B531C9}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="132.86328125" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="132.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,141 +1355,141 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="9">
         <v>2.5</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="9">
         <v>2.5</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="B4" s="11">
         <v>2.5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="11">
         <v>1.5</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="11">
         <v>2.5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" s="11">
         <v>2.5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11">
         <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="13">
         <v>2.5</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="13">
         <v>1.5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="13">
         <v>2.5</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="13">
         <v>2.5</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="B14" s="15">
         <f>SUM(B2:B13)</f>

</xml_diff>